<commit_message>
Anterior a alteração de instrutores por projetos no relatório executivo
</commit_message>
<xml_diff>
--- a/2_consolidado_instrutor_projeto.xlsx
+++ b/2_consolidado_instrutor_projeto.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +446,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>DD2_Onda1</t>
+          <t>DD2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>DD2_Onda2</t>
+          <t>IdearTec1</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>IdearTec_Onda1</t>
+          <t>IdearTec2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>IdearTec_Onda2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -477,22 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -502,22 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -527,22 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
-      </c>
-      <c r="G4" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -555,19 +541,16 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G5" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -577,22 +560,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -605,19 +585,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -627,22 +604,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
-      </c>
-      <c r="G8" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
@@ -655,19 +629,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
-      </c>
-      <c r="G9" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -680,19 +651,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
-      </c>
-      <c r="G10" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
@@ -705,19 +673,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12">
@@ -727,22 +692,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
-      </c>
-      <c r="G12" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
@@ -755,100 +717,88 @@
         <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F13" t="n">
-        <v>6</v>
-      </c>
-      <c r="G13" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ROB_2</t>
+          <t>ROB_10</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ROB_3</t>
+          <t>ROB_11</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F15" t="n">
-        <v>5</v>
-      </c>
-      <c r="G15" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ROB_4</t>
+          <t>ROB_2</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="n">
-        <v>2</v>
-      </c>
-      <c r="G16" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ROB_5</t>
+          <t>ROB_3</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -858,22 +808,19 @@
         <v>4</v>
       </c>
       <c r="D17" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
-        <v>2</v>
-      </c>
-      <c r="G17" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ROB_6</t>
+          <t>ROB_4</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -883,47 +830,41 @@
         <v>6</v>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ROB_7</t>
+          <t>ROB_5</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
-        <v>2</v>
-      </c>
-      <c r="G19" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ROB_8</t>
+          <t>ROB_6</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -933,16 +874,79 @@
         <v>3</v>
       </c>
       <c r="D20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ROB_7</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
         <v>3</v>
       </c>
-      <c r="F20" t="n">
-        <v>3</v>
-      </c>
-      <c r="G20" t="n">
-        <v>11</v>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ROB_8</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>5</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ROB_9</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>5</v>
+      </c>
+      <c r="F23" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Informação de instrutor por projeto
</commit_message>
<xml_diff>
--- a/2_consolidado_instrutor_projeto.xlsx
+++ b/2_consolidado_instrutor_projeto.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,20 +446,40 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>DD2</t>
+          <t>DD2_Onda1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>IdearTec1</t>
+          <t>DD2_Onda2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>IdearTec2</t>
+          <t>DD2_Onda3</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>IT1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>IT2_Onda1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>IT2_Onda2</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>IT2_Onda3</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -472,18 +492,30 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
         <v>14</v>
       </c>
     </row>
@@ -494,18 +526,30 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="n">
         <v>14</v>
       </c>
     </row>
@@ -516,223 +560,343 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_12</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PROG_3</t>
+          <t>PROG_2</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PROG_4</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>3</v>
+      </c>
+      <c r="J7" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PROG_5</t>
+          <t>PROG_4</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>0</v>
       </c>
       <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
         <v>6</v>
       </c>
-      <c r="D8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E8" t="n">
-        <v>6</v>
-      </c>
-      <c r="F8" t="n">
+      <c r="J8" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PROG_6</t>
+          <t>PROG_5</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PROG_7</t>
+          <t>PROG_6</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PROG_8</t>
+          <t>PROG_7</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PROG_9</t>
+          <t>PROG_8</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ROB_1</t>
+          <t>PROG_9</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ROB_10</t>
+          <t>ROB_1</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -742,107 +906,167 @@
         <v>1</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ROB_11</t>
+          <t>ROB_2</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ROB_2</t>
+          <t>ROB_3</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3</v>
+      </c>
+      <c r="J16" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ROB_3</t>
+          <t>ROB_4</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ROB_4</t>
+          <t>ROB_5</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E18" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ROB_5</t>
+          <t>ROB_6</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -855,98 +1079,56 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ROB_6</t>
+          <t>ROB_7</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>ROB_7</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>3</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>4</v>
-      </c>
-      <c r="F21" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>ROB_8</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>5</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>2</v>
-      </c>
-      <c r="F22" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>ROB_9</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" t="n">
-        <v>2</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>5</v>
-      </c>
-      <c r="F23" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>